<commit_message>
New feature is started.
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/List_Discount.xlsx
+++ b/src/test/java/ApachePOI/resource/List_Discount.xlsx
@@ -59,7 +59,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -69,6 +69,33 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="E1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="F1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="G1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="H1" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="I1" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="J1" t="n">
+        <v>9.0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>